<commit_message>
Corrected papon. Updated faculty list page.
</commit_message>
<xml_diff>
--- a/schedule_fall_2025.xlsx
+++ b/schedule_fall_2025.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveumb-my.sharepoint.com/personal/gemma_galecia_umb_edu/Documents/Computer Science/Semester Schedule/2025 Fall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papon/UMass-Boston/umbcs.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{5445D7B3-ADC9-4D92-809B-6BA5AC25F715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B37860E8-94AC-4EC9-9707-0B1E35D6D563}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F31895-6879-DA48-AFE5-E905D5D29A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27C2E1DD-989E-4A3B-9B9F-45BD8BDD6A86}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{27C2E1DD-989E-4A3B-9B9F-45BD8BDD6A86}"/>
   </bookViews>
   <sheets>
     <sheet name="CLSSCHED2 (004)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="190">
   <si>
     <t>Sect</t>
   </si>
@@ -587,6 +600,9 @@
   </si>
   <si>
     <t>College of Management</t>
+  </si>
+  <si>
+    <t>Papon, Tarikul Islam</t>
   </si>
 </sst>
 </file>
@@ -1450,24 +1466,24 @@
   <dimension ref="A1:J174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1499,7 +1515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +1550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1604,7 +1620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1639,7 +1655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1709,7 +1725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1744,7 +1760,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1779,7 +1795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1814,7 +1830,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1849,7 +1865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1884,7 +1900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1954,7 +1970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1989,7 +2005,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2024,7 +2040,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2059,7 +2075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2094,7 +2110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -2129,7 +2145,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2164,7 +2180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2199,7 +2215,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2234,7 +2250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2269,7 +2285,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2300,8 +2316,11 @@
       <c r="I24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2336,7 +2355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2403,7 +2422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2438,7 +2457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2473,7 +2492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2508,7 +2527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2543,7 +2562,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2575,7 +2594,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2610,7 +2629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2645,7 +2664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2680,7 +2699,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2715,7 +2734,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2747,7 +2766,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2779,7 +2798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2814,7 +2833,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2849,7 +2868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2919,7 +2938,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2954,7 +2973,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2989,7 +3008,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -3024,7 +3043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -3059,7 +3078,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3094,7 +3113,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3129,7 +3148,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -3164,7 +3183,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -3199,7 +3218,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -3234,7 +3253,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -3269,7 +3288,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -3304,7 +3323,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3339,7 +3358,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3374,7 +3393,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3428,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -3444,7 +3463,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3479,7 +3498,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3514,7 +3533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3549,7 +3568,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3584,7 +3603,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3619,7 +3638,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3654,7 +3673,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3689,7 +3708,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3724,7 +3743,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3759,7 +3778,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3794,7 +3813,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3829,7 +3848,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -3864,7 +3883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3899,7 +3918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -3934,7 +3953,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -3969,7 +3988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -4004,7 +4023,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -4039,7 +4058,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -4074,7 +4093,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -4103,7 +4122,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4132,7 +4151,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -4161,7 +4180,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -4190,7 +4209,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -4219,7 +4238,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -4248,7 +4267,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -4277,7 +4296,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4306,7 +4325,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -4332,7 +4351,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -4361,7 +4380,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -4390,7 +4409,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -4425,7 +4444,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -4460,7 +4479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -4495,7 +4514,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -4530,7 +4549,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -4565,7 +4584,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -4600,7 +4619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -4635,7 +4654,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -4670,7 +4689,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -4705,7 +4724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -4740,7 +4759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -4775,7 +4794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -4810,7 +4829,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4845,7 +4864,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -4880,7 +4899,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4915,7 +4934,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -4944,7 +4963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -4973,7 +4992,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -5002,7 +5021,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -5031,7 +5050,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -5060,7 +5079,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -5086,7 +5105,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -5115,7 +5134,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -5144,7 +5163,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -5173,7 +5192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -5202,7 +5221,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>10</v>
       </c>
@@ -5231,7 +5250,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -5260,7 +5279,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -5289,7 +5308,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -5318,7 +5337,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -5347,7 +5366,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -5376,7 +5395,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -5402,7 +5421,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -5428,7 +5447,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -5454,7 +5473,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -5489,7 +5508,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -5518,7 +5537,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -5547,7 +5566,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>10</v>
       </c>
@@ -5576,7 +5595,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -5605,7 +5624,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>10</v>
       </c>
@@ -5634,7 +5653,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -5663,7 +5682,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>10</v>
       </c>
@@ -5692,7 +5711,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>10</v>
       </c>
@@ -5721,7 +5740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -5750,7 +5769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>10</v>
       </c>
@@ -5779,7 +5798,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>10</v>
       </c>
@@ -5808,7 +5827,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -5843,7 +5862,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -5875,7 +5894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -5910,7 +5929,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -5945,7 +5964,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -5974,7 +5993,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -6009,7 +6028,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>149</v>
       </c>
@@ -6044,7 +6063,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -6079,7 +6098,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>149</v>
       </c>
@@ -6114,7 +6133,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -6149,7 +6168,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -6184,7 +6203,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>149</v>
       </c>
@@ -6219,7 +6238,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>149</v>
       </c>
@@ -6248,7 +6267,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -6283,7 +6302,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>149</v>
       </c>
@@ -6318,7 +6337,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -6353,7 +6372,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -6388,7 +6407,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -6417,7 +6436,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -6452,7 +6471,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>149</v>
       </c>
@@ -6487,7 +6506,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -6522,7 +6541,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>149</v>
       </c>
@@ -6557,7 +6576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>149</v>
       </c>
@@ -6592,7 +6611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>149</v>
       </c>
@@ -6627,7 +6646,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>149</v>
       </c>
@@ -6662,7 +6681,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>149</v>
       </c>
@@ -6691,7 +6710,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>149</v>
       </c>
@@ -6726,7 +6745,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>149</v>
       </c>
@@ -6761,7 +6780,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>149</v>
       </c>
@@ -6796,7 +6815,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>149</v>
       </c>
@@ -6831,7 +6850,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>149</v>
       </c>
@@ -6866,7 +6885,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>149</v>
       </c>
@@ -6901,7 +6920,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>149</v>
       </c>
@@ -6936,7 +6955,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>149</v>
       </c>
@@ -6971,7 +6990,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>149</v>
       </c>
@@ -7000,7 +7019,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>149</v>
       </c>
@@ -7035,7 +7054,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>149</v>
       </c>
@@ -7070,7 +7089,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>149</v>
       </c>
@@ -7105,7 +7124,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>149</v>
       </c>
@@ -7140,7 +7159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>149</v>
       </c>
@@ -7175,7 +7194,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>149</v>
       </c>
@@ -7210,7 +7229,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>149</v>
       </c>

</xml_diff>